<commit_message>
- Added Delete Function
</commit_message>
<xml_diff>
--- a/data_input.xlsx
+++ b/data_input.xlsx
@@ -8,24 +8,31 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\working\My Project\automationshopify\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{384BFC69-A3A0-44C7-84D8-D794BF8725D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A609859D-0B4D-4DFC-8A6D-D5C3E65FD0E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2850" yWindow="0" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="34">
   <si>
     <t>email</t>
   </si>
@@ -36,15 +43,9 @@
     <t>name</t>
   </si>
   <si>
-    <t>john9901@gmail.com</t>
-  </si>
-  <si>
     <t>john123</t>
   </si>
   <si>
-    <t>john9901</t>
-  </si>
-  <si>
     <t>fname</t>
   </si>
   <si>
@@ -70,13 +71,76 @@
   </si>
   <si>
     <t>doe</t>
+  </si>
+  <si>
+    <t>luxemburg</t>
+  </si>
+  <si>
+    <t>this street</t>
+  </si>
+  <si>
+    <t>Lampung</t>
+  </si>
+  <si>
+    <t>+6281000008</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>Indonesia</t>
+  </si>
+  <si>
+    <t>john9935@gmail.com</t>
+  </si>
+  <si>
+    <t>john9935</t>
+  </si>
+  <si>
+    <t>john9936</t>
+  </si>
+  <si>
+    <t>john9936@gmail.com</t>
+  </si>
+  <si>
+    <t>+6281000009</t>
+  </si>
+  <si>
+    <t>john9937</t>
+  </si>
+  <si>
+    <t>john9938</t>
+  </si>
+  <si>
+    <t>john9939</t>
+  </si>
+  <si>
+    <t>john9940</t>
+  </si>
+  <si>
+    <t>john9941</t>
+  </si>
+  <si>
+    <t>john9941@gmail.com</t>
+  </si>
+  <si>
+    <t>john9937@gmail.com</t>
+  </si>
+  <si>
+    <t>john9938@gmail.com</t>
+  </si>
+  <si>
+    <t>john9939@gmail.com</t>
+  </si>
+  <si>
+    <t>john9940@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,6 +152,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -114,9 +184,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -398,20 +470,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -421,48 +496,287 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="J1" t="s">
+      <c r="E2" t="s">
         <v>12</v>
       </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2">
+        <v>35111</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H3" t="s">
         <v>14</v>
+      </c>
+      <c r="I3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3">
+        <v>35112</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4">
+        <v>35113</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5">
+        <v>35114</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6">
+        <v>35115</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7">
+        <v>35116</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8">
+        <v>35117</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{BA5779C8-2C68-42F9-BB34-67075314C543}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{C3871D8E-4C43-46D3-8BD0-D543D37EEABA}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{F8C7C7ED-6716-4460-B253-30623D9F1420}"/>
+    <hyperlink ref="A6" r:id="rId4" xr:uid="{E7513E2D-DA4A-4D60-B628-7029E115FD0F}"/>
+    <hyperlink ref="A8" r:id="rId5" xr:uid="{2A88994A-7F12-42FB-877C-AC9E99360FFE}"/>
+    <hyperlink ref="A5" r:id="rId6" xr:uid="{C27563C2-0462-41BB-90F4-1D00574DD067}"/>
+    <hyperlink ref="A7" r:id="rId7" xr:uid="{653CF5F6-D3F1-4CFC-91AB-E6E28EDC9805}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>